<commit_message>
Can now create sale offer for Destock user
Envoyé depuis mon iPhone.
P.S. : Ce commit est certifié sans gluten
</commit_message>
<xml_diff>
--- a/tests/resources/integration_annonce_pharmacie.xlsx
+++ b/tests/resources/integration_annonce_pharmacie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerylcdp/PycharmProjects/importApp/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A22D6C-12BD-5942-999D-C020ECD5D3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B59AE53-1281-DA4D-A488-2CE78DF440E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36440" yWindow="2040" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Complément alimentaire</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>LEKEO1</t>
+  </si>
+  <si>
+    <t>Sans reference annonce 2</t>
+  </si>
+  <si>
+    <t>Mon lot 2</t>
   </si>
 </sst>
 </file>
@@ -4103,7 +4109,7 @@
   <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4375,22 +4381,47 @@
         <v>999</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
+    <row r="7" spans="1:26" s="61" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="74">
+        <v>47788</v>
+      </c>
+      <c r="K7" s="21">
+        <v>10</v>
+      </c>
+      <c r="L7" s="21">
+        <v>20</v>
+      </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="26"/>
+      <c r="N7" s="25">
+        <v>10</v>
+      </c>
+      <c r="O7" s="26">
+        <v>999</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
@@ -4429,7 +4460,6 @@
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
       <c r="D10" s="30"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
@@ -18980,8 +19010,8 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" sqref="L4:N1018" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CIP/ACL ou EAN - Veuillez saisir un code à 13 caractères" sqref="B7:B1018" xr:uid="{00000000-0002-0000-0100-000005000000}">
-      <formula1>AND(GTE(LEN(B7),MIN((1),(13))),LTE(LEN(B7),MAX((1),(13))))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="CIP/ACL ou EAN - Veuillez saisir un code à 13 caractères" sqref="B8:B1018" xr:uid="{00000000-0002-0000-0100-000005000000}">
+      <formula1>AND(GTE(LEN(B8),MIN((1),(13))),LTE(LEN(B8),MAX((1),(13))))</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Classement produit - Veuillez saisir un chiffre supérieur ou égale à 1" sqref="A4:A1018" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>1</formula1>
@@ -19067,7 +19097,7 @@
       </c>
       <c r="C2" s="72">
         <f ca="1">TODAY()</f>
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>

</xml_diff>